<commit_message>
Detect when conviction occurred after 11/9/2016
[#167685800]
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="51200" windowHeight="28800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="294">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -886,6 +886,21 @@
   </si>
   <si>
     <t>Dismiss all HS 11357 convictions</t>
+  </si>
+  <si>
+    <t>Occurred after 11/9/2016</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TROY, CASTOR</t>
+  </si>
+  <si>
+    <t>02/14/2017</t>
+  </si>
+  <si>
+    <t>2.7</t>
   </si>
 </sst>
 </file>
@@ -924,7 +939,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -965,6 +980,18 @@
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1111,7 +1138,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1379,8 +1406,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1510,8 +1567,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1556,6 +1634,11 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1600,6 +1683,11 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2758,12 +2846,12 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DH39"/>
+  <dimension ref="A1:DI40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CR1" workbookViewId="0">
-      <pane ySplit="1200" activePane="bottomLeft"/>
-      <selection activeCell="BB1" sqref="BB1"/>
-      <selection pane="bottomLeft" activeCell="CZ17" sqref="CZ17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CJ1" workbookViewId="0">
+      <pane ySplit="1200" topLeftCell="A5" activePane="bottomLeft"/>
+      <selection activeCell="CU2" sqref="CU2"/>
+      <selection pane="bottomLeft" activeCell="DB45" sqref="DB45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2857,17 +2945,17 @@
     <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
     <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
     <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
-    <col min="98" max="98" width="24" style="1" customWidth="1"/>
-    <col min="99" max="101" width="23.6640625" style="1" customWidth="1"/>
-    <col min="102" max="102" width="12.5" style="1" customWidth="1"/>
-    <col min="103" max="103" width="23.5" style="1" customWidth="1"/>
-    <col min="104" max="104" width="23.1640625" style="1" customWidth="1"/>
-    <col min="105" max="109" width="20.5" style="1" customWidth="1"/>
-    <col min="110" max="111" width="25.83203125" style="1" customWidth="1"/>
-    <col min="112" max="112" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="24" style="1" customWidth="1"/>
+    <col min="100" max="102" width="23.6640625" style="1" customWidth="1"/>
+    <col min="103" max="103" width="12.5" style="1" customWidth="1"/>
+    <col min="104" max="104" width="23.5" style="1" customWidth="1"/>
+    <col min="105" max="105" width="23.1640625" style="1" customWidth="1"/>
+    <col min="106" max="110" width="20.5" style="1" customWidth="1"/>
+    <col min="111" max="112" width="25.83203125" style="1" customWidth="1"/>
+    <col min="113" max="113" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" s="42" customFormat="1" ht="27.75" customHeight="1">
+    <row r="1" spans="1:113" s="42" customFormat="1" ht="27.75" customHeight="1">
       <c r="B1" s="39" t="s">
         <v>253</v>
       </c>
@@ -3053,8 +3141,11 @@
       <c r="DH1" s="41" t="s">
         <v>252</v>
       </c>
+      <c r="DI1" s="41" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="2" spans="1:112" ht="20.25" customHeight="1">
+    <row r="2" spans="1:113" ht="20.25" customHeight="1">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3350,49 +3441,52 @@
         <v>96</v>
       </c>
       <c r="CU2" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="CV2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CV2" s="2" t="s">
+      <c r="CW2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CW2" s="2" t="s">
+      <c r="CX2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CX2" s="2" t="s">
+      <c r="CY2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CY2" s="2" t="s">
+      <c r="CZ2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="CZ2" s="2" t="s">
+      <c r="DA2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="DA2" s="2" t="s">
+      <c r="DB2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="DB2" s="2" t="s">
+      <c r="DC2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DD2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="DE2" s="2" t="s">
+      <c r="DF2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="DF2" s="2" t="s">
+      <c r="DG2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DG2" s="2" t="s">
+      <c r="DH2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DH2" s="2" t="s">
+      <c r="DI2" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:112" ht="20.25" customHeight="1">
+    <row r="3" spans="1:113" ht="20.25" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
@@ -3609,11 +3703,12 @@
       <c r="DC3" s="6"/>
       <c r="DD3" s="6"/>
       <c r="DE3" s="6"/>
-      <c r="DF3" s="7"/>
+      <c r="DF3" s="6"/>
       <c r="DG3" s="7"/>
       <c r="DH3" s="7"/>
+      <c r="DI3" s="7"/>
     </row>
-    <row r="4" spans="1:112" ht="20" customHeight="1">
+    <row r="4" spans="1:113" ht="20" customHeight="1">
       <c r="B4" s="8" t="s">
         <v>107</v>
       </c>
@@ -3840,11 +3935,12 @@
       <c r="DC4" s="11"/>
       <c r="DD4" s="11"/>
       <c r="DE4" s="11"/>
-      <c r="DF4" s="12"/>
+      <c r="DF4" s="11"/>
       <c r="DG4" s="12"/>
       <c r="DH4" s="12"/>
+      <c r="DI4" s="12"/>
     </row>
-    <row r="5" spans="1:112" ht="20" customHeight="1">
+    <row r="5" spans="1:113" ht="20" customHeight="1">
       <c r="B5" s="8" t="s">
         <v>107</v>
       </c>
@@ -4061,11 +4157,12 @@
       <c r="DC5" s="11"/>
       <c r="DD5" s="11"/>
       <c r="DE5" s="11"/>
-      <c r="DF5" s="12"/>
+      <c r="DF5" s="11"/>
       <c r="DG5" s="12"/>
       <c r="DH5" s="12"/>
+      <c r="DI5" s="12"/>
     </row>
-    <row r="6" spans="1:112" ht="20" customHeight="1">
+    <row r="6" spans="1:113" ht="20" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4282,11 +4379,12 @@
       <c r="DC6" s="11"/>
       <c r="DD6" s="11"/>
       <c r="DE6" s="11"/>
-      <c r="DF6" s="12"/>
+      <c r="DF6" s="11"/>
       <c r="DG6" s="12"/>
       <c r="DH6" s="12"/>
+      <c r="DI6" s="12"/>
     </row>
-    <row r="7" spans="1:112" ht="20" customHeight="1">
+    <row r="7" spans="1:113" ht="20" customHeight="1">
       <c r="B7" s="8" t="s">
         <v>107</v>
       </c>
@@ -4503,11 +4601,12 @@
       <c r="DC7" s="11"/>
       <c r="DD7" s="11"/>
       <c r="DE7" s="11"/>
-      <c r="DF7" s="12"/>
+      <c r="DF7" s="11"/>
       <c r="DG7" s="12"/>
       <c r="DH7" s="12"/>
+      <c r="DI7" s="12"/>
     </row>
-    <row r="8" spans="1:112" ht="20" customHeight="1">
+    <row r="8" spans="1:113" ht="20" customHeight="1">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -4731,7 +4830,7 @@
         <v>145</v>
       </c>
       <c r="CU8" s="11" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV8" s="11" t="s">
         <v>146</v>
@@ -4740,40 +4839,43 @@
         <v>146</v>
       </c>
       <c r="CX8" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY8" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="CY8" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="CZ8" s="11" t="s">
         <v>148</v>
       </c>
       <c r="DA8" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="DB8" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="DB8" s="11" t="s">
+      <c r="DC8" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="DC8" s="11" t="s">
+      <c r="DD8" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="DD8" s="11" t="s">
-        <v>270</v>
       </c>
       <c r="DE8" s="11" t="s">
         <v>270</v>
       </c>
       <c r="DF8" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="DG8" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="DG8" s="11" t="s">
+      <c r="DH8" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="DH8" s="11" t="s">
+      <c r="DI8" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:112" ht="20" customHeight="1">
+    <row r="9" spans="1:113" ht="20" customHeight="1">
       <c r="B9" s="23" t="s">
         <v>107</v>
       </c>
@@ -4993,8 +5095,9 @@
       <c r="DF9" s="26"/>
       <c r="DG9" s="26"/>
       <c r="DH9" s="26"/>
+      <c r="DI9" s="26"/>
     </row>
-    <row r="10" spans="1:112" ht="20" customHeight="1">
+    <row r="10" spans="1:113" ht="20" customHeight="1">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -5218,49 +5321,52 @@
         <v>156</v>
       </c>
       <c r="CU10" s="26" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV10" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CW10" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CX10" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="CX10" s="26" t="s">
+      <c r="CY10" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="CY10" s="26" t="s">
+      <c r="CZ10" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="CZ10" s="26" t="s">
+      <c r="DA10" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="DA10" s="26" t="s">
+      <c r="DB10" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="DB10" s="26" t="s">
+      <c r="DC10" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DC10" s="26" t="s">
+      <c r="DD10" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DD10" s="26" t="s">
+      <c r="DE10" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DE10" s="26" t="s">
+      <c r="DF10" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DF10" s="26" t="s">
+      <c r="DG10" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG10" s="26" t="s">
+      <c r="DH10" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DH10" s="26" t="s">
+      <c r="DI10" s="26" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:112" ht="20" customHeight="1">
+    <row r="11" spans="1:113" ht="20" customHeight="1">
       <c r="B11" s="23" t="s">
         <v>107</v>
       </c>
@@ -5476,8 +5582,9 @@
       <c r="DF11" s="26"/>
       <c r="DG11" s="26"/>
       <c r="DH11" s="26"/>
+      <c r="DI11" s="26"/>
     </row>
-    <row r="12" spans="1:112" ht="20" customHeight="1">
+    <row r="12" spans="1:113" ht="20" customHeight="1">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -5701,49 +5808,52 @@
         <v>156</v>
       </c>
       <c r="CU12" s="26" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV12" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CW12" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CX12" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="CX12" s="26" t="s">
+      <c r="CY12" s="26" t="s">
         <v>256</v>
-      </c>
-      <c r="CY12" s="26" t="s">
-        <v>255</v>
       </c>
       <c r="CZ12" s="26" t="s">
         <v>255</v>
       </c>
       <c r="DA12" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="DB12" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="DB12" s="26" t="s">
+      <c r="DC12" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DC12" s="26" t="s">
+      <c r="DD12" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DD12" s="26" t="s">
+      <c r="DE12" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DE12" s="26" t="s">
+      <c r="DF12" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DF12" s="26" t="s">
+      <c r="DG12" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG12" s="26" t="s">
+      <c r="DH12" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DH12" s="26" t="s">
+      <c r="DI12" s="26" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="13" spans="1:112" ht="20" customHeight="1">
+    <row r="13" spans="1:113" ht="20" customHeight="1">
       <c r="B13" s="23" t="s">
         <v>107</v>
       </c>
@@ -5967,8 +6077,9 @@
       <c r="DF13" s="26"/>
       <c r="DG13" s="26"/>
       <c r="DH13" s="26"/>
+      <c r="DI13" s="26"/>
     </row>
-    <row r="14" spans="1:112" ht="20" customHeight="1">
+    <row r="14" spans="1:113" ht="20" customHeight="1">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -6194,7 +6305,7 @@
         <v>169</v>
       </c>
       <c r="CU14" s="16" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV14" s="16" t="s">
         <v>146</v>
@@ -6203,40 +6314,43 @@
         <v>146</v>
       </c>
       <c r="CX14" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY14" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="CY14" s="16" t="s">
+      <c r="CZ14" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="CZ14" s="16" t="s">
+      <c r="DA14" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="DA14" s="16" t="s">
+      <c r="DB14" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="DB14" s="16" t="s">
+      <c r="DC14" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DC14" s="16" t="s">
+      <c r="DD14" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="DD14" s="16" t="s">
+      <c r="DE14" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DE14" s="16" t="s">
+      <c r="DF14" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DF14" s="16" t="s">
+      <c r="DG14" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DG14" s="17" t="s">
+      <c r="DH14" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="DH14" s="17" t="s">
+      <c r="DI14" s="17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:112" ht="20" customHeight="1">
+    <row r="15" spans="1:113" ht="20" customHeight="1">
       <c r="B15" s="13" t="s">
         <v>107</v>
       </c>
@@ -6463,11 +6577,12 @@
       <c r="DC15" s="16"/>
       <c r="DD15" s="16"/>
       <c r="DE15" s="16"/>
-      <c r="DF15" s="17"/>
+      <c r="DF15" s="16"/>
       <c r="DG15" s="17"/>
       <c r="DH15" s="17"/>
+      <c r="DI15" s="17"/>
     </row>
-    <row r="16" spans="1:112" ht="20" customHeight="1">
+    <row r="16" spans="1:113" ht="20" customHeight="1">
       <c r="B16" s="13" t="s">
         <v>107</v>
       </c>
@@ -6694,11 +6809,12 @@
       <c r="DC16" s="16"/>
       <c r="DD16" s="16"/>
       <c r="DE16" s="16"/>
-      <c r="DF16" s="17"/>
+      <c r="DF16" s="16"/>
       <c r="DG16" s="17"/>
       <c r="DH16" s="17"/>
+      <c r="DI16" s="17"/>
     </row>
-    <row r="17" spans="1:112" ht="20" customHeight="1">
+    <row r="17" spans="1:113" ht="20" customHeight="1">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -6922,7 +7038,7 @@
         <v>169</v>
       </c>
       <c r="CU17" s="16" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV17" s="16" t="s">
         <v>146</v>
@@ -6931,40 +7047,43 @@
         <v>146</v>
       </c>
       <c r="CX17" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY17" s="16" t="s">
         <v>258</v>
-      </c>
-      <c r="CY17" s="16" t="s">
-        <v>257</v>
       </c>
       <c r="CZ17" s="16" t="s">
         <v>257</v>
       </c>
       <c r="DA17" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="DB17" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="DB17" s="16" t="s">
+      <c r="DC17" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DC17" s="16" t="s">
+      <c r="DD17" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="DD17" s="16" t="s">
+      <c r="DE17" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DE17" s="16" t="s">
+      <c r="DF17" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DF17" s="16" t="s">
+      <c r="DG17" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DG17" s="17" t="s">
+      <c r="DH17" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="DH17" s="17" t="s">
+      <c r="DI17" s="17" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="18" spans="1:112" ht="20" customHeight="1">
+    <row r="18" spans="1:113" ht="20" customHeight="1">
       <c r="B18" s="13" t="s">
         <v>107</v>
       </c>
@@ -7189,11 +7308,12 @@
       <c r="DC18" s="16"/>
       <c r="DD18" s="16"/>
       <c r="DE18" s="16"/>
-      <c r="DF18" s="17"/>
+      <c r="DF18" s="16"/>
       <c r="DG18" s="17"/>
       <c r="DH18" s="17"/>
+      <c r="DI18" s="17"/>
     </row>
-    <row r="19" spans="1:112" ht="20" customHeight="1">
+    <row r="19" spans="1:113" ht="20" customHeight="1">
       <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
@@ -7420,11 +7540,12 @@
       <c r="DC19" s="21"/>
       <c r="DD19" s="21"/>
       <c r="DE19" s="21"/>
-      <c r="DF19" s="22"/>
+      <c r="DF19" s="21"/>
       <c r="DG19" s="22"/>
       <c r="DH19" s="22"/>
+      <c r="DI19" s="22"/>
     </row>
-    <row r="20" spans="1:112" ht="20" customHeight="1">
+    <row r="20" spans="1:113" ht="20" customHeight="1">
       <c r="A20" t="b">
         <v>1</v>
       </c>
@@ -7642,49 +7763,52 @@
         <v>169</v>
       </c>
       <c r="CU20" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CV20" s="21" t="s">
+      <c r="CW20" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="CW20" s="21" t="s">
+      <c r="CX20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CX20" s="21" t="s">
+      <c r="CY20" s="21" t="s">
         <v>266</v>
-      </c>
-      <c r="CY20" s="21" t="s">
-        <v>267</v>
       </c>
       <c r="CZ20" s="21" t="s">
         <v>267</v>
       </c>
       <c r="DA20" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="DB20" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="DB20" s="21" t="s">
+      <c r="DC20" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="DC20" s="21" t="s">
-        <v>149</v>
       </c>
       <c r="DD20" s="21" t="s">
         <v>149</v>
       </c>
       <c r="DE20" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DF20" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="DF20" s="21" t="s">
+      <c r="DG20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DG20" s="22" t="s">
+      <c r="DH20" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DH20" s="22" t="s">
+      <c r="DI20" s="22" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:112" ht="20" customHeight="1">
+    <row r="21" spans="1:113" ht="20" customHeight="1">
       <c r="B21" s="18" t="s">
         <v>107</v>
       </c>
@@ -7911,11 +8035,12 @@
       <c r="DC21" s="21"/>
       <c r="DD21" s="21"/>
       <c r="DE21" s="21"/>
-      <c r="DF21" s="22"/>
+      <c r="DF21" s="21"/>
       <c r="DG21" s="22"/>
       <c r="DH21" s="22"/>
+      <c r="DI21" s="22"/>
     </row>
-    <row r="22" spans="1:112" ht="20" customHeight="1">
+    <row r="22" spans="1:113" ht="20" customHeight="1">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -8139,49 +8264,52 @@
         <v>169</v>
       </c>
       <c r="CU22" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CV22" s="21" t="s">
+      <c r="CW22" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="CW22" s="21" t="s">
+      <c r="CX22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CX22" s="21" t="s">
+      <c r="CY22" s="21" t="s">
         <v>266</v>
-      </c>
-      <c r="CY22" s="21" t="s">
-        <v>267</v>
       </c>
       <c r="CZ22" s="21" t="s">
         <v>267</v>
       </c>
       <c r="DA22" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="DB22" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="DB22" s="21" t="s">
+      <c r="DC22" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="DC22" s="21" t="s">
-        <v>149</v>
       </c>
       <c r="DD22" s="21" t="s">
         <v>149</v>
       </c>
       <c r="DE22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DF22" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="DF22" s="21" t="s">
+      <c r="DG22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DG22" s="22" t="s">
+      <c r="DH22" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DH22" s="22" t="s">
+      <c r="DI22" s="22" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:112" ht="20" customHeight="1">
+    <row r="23" spans="1:113" ht="20" customHeight="1">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -8401,28 +8529,28 @@
         <v>189</v>
       </c>
       <c r="CU23" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV23" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="CV23" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CW23" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CX23" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY23" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="CY23" s="26" t="s">
+      <c r="CZ23" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="CZ23" s="26" t="s">
+      <c r="DA23" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="DA23" s="26" t="s">
+      <c r="DB23" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="DB23" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="DC23" s="26" t="s">
         <v>149</v>
@@ -8431,19 +8559,22 @@
         <v>149</v>
       </c>
       <c r="DE23" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DF23" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DF23" s="26" t="s">
+      <c r="DG23" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG23" s="27" t="s">
+      <c r="DH23" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="DH23" s="27" t="s">
+      <c r="DI23" s="27" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="24" spans="1:112" ht="20" customHeight="1">
+    <row r="24" spans="1:113" ht="20" customHeight="1">
       <c r="B24" s="23" t="s">
         <v>107</v>
       </c>
@@ -8666,11 +8797,12 @@
       <c r="DC24" s="26"/>
       <c r="DD24" s="26"/>
       <c r="DE24" s="26"/>
-      <c r="DF24" s="27"/>
+      <c r="DF24" s="26"/>
       <c r="DG24" s="27"/>
       <c r="DH24" s="27"/>
+      <c r="DI24" s="27"/>
     </row>
-    <row r="25" spans="1:112" ht="20" customHeight="1">
+    <row r="25" spans="1:113" ht="20" customHeight="1">
       <c r="B25" s="23" t="s">
         <v>107</v>
       </c>
@@ -8879,11 +9011,12 @@
       <c r="DC25" s="26"/>
       <c r="DD25" s="26"/>
       <c r="DE25" s="26"/>
-      <c r="DF25" s="27"/>
+      <c r="DF25" s="26"/>
       <c r="DG25" s="27"/>
       <c r="DH25" s="27"/>
+      <c r="DI25" s="27"/>
     </row>
-    <row r="26" spans="1:112" ht="20" customHeight="1">
+    <row r="26" spans="1:113" ht="20" customHeight="1">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -9091,28 +9224,28 @@
         <v>189</v>
       </c>
       <c r="CU26" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV26" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="CV26" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CW26" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CX26" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY26" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="CY26" s="26" t="s">
+      <c r="CZ26" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="CZ26" s="26" t="s">
+      <c r="DA26" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="DA26" s="26" t="s">
+      <c r="DB26" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="DB26" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="DC26" s="26" t="s">
         <v>149</v>
@@ -9121,19 +9254,22 @@
         <v>149</v>
       </c>
       <c r="DE26" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DF26" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DF26" s="26" t="s">
+      <c r="DG26" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG26" s="26" t="s">
+      <c r="DH26" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DH26" s="26" t="s">
+      <c r="DI26" s="26" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:112" ht="20" customHeight="1">
+    <row r="27" spans="1:113" ht="20" customHeight="1">
       <c r="A27" t="b">
         <v>1</v>
       </c>
@@ -9341,28 +9477,28 @@
         <v>189</v>
       </c>
       <c r="CU27" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV27" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="CV27" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CW27" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CX27" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY27" s="26" t="s">
         <v>199</v>
-      </c>
-      <c r="CY27" s="26" t="s">
-        <v>193</v>
       </c>
       <c r="CZ27" s="26" t="s">
         <v>193</v>
       </c>
       <c r="DA27" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="DB27" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="DB27" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="DC27" s="26" t="s">
         <v>149</v>
@@ -9371,19 +9507,22 @@
         <v>149</v>
       </c>
       <c r="DE27" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DF27" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DF27" s="26" t="s">
+      <c r="DG27" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG27" s="26" t="s">
+      <c r="DH27" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="DH27" s="26" t="s">
+      <c r="DI27" s="26" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:112" ht="20" customHeight="1">
+    <row r="28" spans="1:113" ht="20" customHeight="1">
       <c r="A28" t="b">
         <v>1</v>
       </c>
@@ -9607,7 +9746,7 @@
         <v>156</v>
       </c>
       <c r="CU28" s="31" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV28" s="31" t="s">
         <v>146</v>
@@ -9616,40 +9755,43 @@
         <v>146</v>
       </c>
       <c r="CX28" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY28" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="CY28" s="31" t="s">
+      <c r="CZ28" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="CZ28" s="31" t="s">
+      <c r="DA28" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="DA28" s="31" t="s">
+      <c r="DB28" s="31" t="s">
         <v>156</v>
-      </c>
-      <c r="DB28" s="31" t="s">
-        <v>270</v>
       </c>
       <c r="DC28" s="31" t="s">
         <v>270</v>
       </c>
       <c r="DD28" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="DE28" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="DE28" s="31" t="s">
+      <c r="DF28" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="DF28" s="31" t="s">
+      <c r="DG28" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="DG28" s="31" t="s">
+      <c r="DH28" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="DH28" s="31" t="s">
+      <c r="DI28" s="31" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:112" ht="20" customHeight="1">
+    <row r="29" spans="1:113" ht="20" customHeight="1">
       <c r="B29" s="28" t="s">
         <v>107</v>
       </c>
@@ -9876,11 +10018,12 @@
       <c r="DC29" s="31"/>
       <c r="DD29" s="31"/>
       <c r="DE29" s="31"/>
-      <c r="DF29" s="32"/>
+      <c r="DF29" s="31"/>
       <c r="DG29" s="32"/>
       <c r="DH29" s="32"/>
+      <c r="DI29" s="32"/>
     </row>
-    <row r="30" spans="1:112" ht="20" customHeight="1">
+    <row r="30" spans="1:113" ht="20" customHeight="1">
       <c r="A30" t="b">
         <v>1</v>
       </c>
@@ -10104,7 +10247,7 @@
         <v>156</v>
       </c>
       <c r="CU30" s="31" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV30" s="31" t="s">
         <v>146</v>
@@ -10113,40 +10256,43 @@
         <v>146</v>
       </c>
       <c r="CX30" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY30" s="31" t="s">
         <v>208</v>
-      </c>
-      <c r="CY30" s="31" t="s">
-        <v>206</v>
       </c>
       <c r="CZ30" s="31" t="s">
         <v>206</v>
       </c>
       <c r="DA30" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="DB30" s="31" t="s">
         <v>156</v>
-      </c>
-      <c r="DB30" s="31" t="s">
-        <v>270</v>
       </c>
       <c r="DC30" s="31" t="s">
         <v>270</v>
       </c>
       <c r="DD30" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="DE30" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="DE30" s="31" t="s">
+      <c r="DF30" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="DF30" s="31" t="s">
+      <c r="DG30" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="DG30" s="31" t="s">
+      <c r="DH30" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="DH30" s="31" t="s">
+      <c r="DI30" s="31" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:112" ht="20" customHeight="1">
+    <row r="31" spans="1:113" ht="20" customHeight="1">
       <c r="A31" t="b">
         <v>1</v>
       </c>
@@ -10370,49 +10516,52 @@
         <v>145</v>
       </c>
       <c r="CU31" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="CV31" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="CV31" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="CW31" s="11" t="s">
         <v>146</v>
       </c>
       <c r="CX31" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY31" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="CY31" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="CZ31" s="11" t="s">
         <v>205</v>
       </c>
       <c r="DA31" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="DB31" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="DB31" s="11" t="s">
+      <c r="DC31" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="DC31" s="11" t="s">
+      <c r="DD31" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="DD31" s="11" t="s">
-        <v>270</v>
       </c>
       <c r="DE31" s="11" t="s">
         <v>270</v>
       </c>
       <c r="DF31" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="DG31" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="DG31" s="11" t="s">
+      <c r="DH31" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="DH31" s="11" t="s">
+      <c r="DI31" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:112" ht="20" customHeight="1">
+    <row r="32" spans="1:113" ht="20" customHeight="1">
       <c r="B32" s="8" t="s">
         <v>107</v>
       </c>
@@ -10639,11 +10788,12 @@
       <c r="DC32" s="11"/>
       <c r="DD32" s="11"/>
       <c r="DE32" s="11"/>
-      <c r="DF32" s="12"/>
+      <c r="DF32" s="11"/>
       <c r="DG32" s="12"/>
       <c r="DH32" s="12"/>
+      <c r="DI32" s="12"/>
     </row>
-    <row r="33" spans="1:112" ht="20" customHeight="1">
+    <row r="33" spans="1:113" ht="20" customHeight="1">
       <c r="A33" t="b">
         <v>1</v>
       </c>
@@ -10857,7 +11007,7 @@
         <v>149</v>
       </c>
       <c r="CU33" s="26" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV33" s="26" t="s">
         <v>146</v>
@@ -10866,40 +11016,43 @@
         <v>146</v>
       </c>
       <c r="CX33" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY33" s="26" t="s">
         <v>215</v>
-      </c>
-      <c r="CY33" s="26" t="s">
-        <v>216</v>
       </c>
       <c r="CZ33" s="26" t="s">
         <v>216</v>
       </c>
       <c r="DA33" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="DB33" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DB33" s="26" t="s">
+      <c r="DC33" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DC33" s="26" t="s">
+      <c r="DD33" s="26" t="s">
         <v>149</v>
-      </c>
-      <c r="DD33" s="26" t="s">
-        <v>270</v>
       </c>
       <c r="DE33" s="26" t="s">
         <v>270</v>
       </c>
       <c r="DF33" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="DG33" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG33" s="26" t="s">
+      <c r="DH33" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DH33" s="26" t="s">
+      <c r="DI33" s="26" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:112" ht="20" customHeight="1">
+    <row r="34" spans="1:113" ht="20" customHeight="1">
       <c r="A34" t="b">
         <v>1</v>
       </c>
@@ -11115,7 +11268,7 @@
         <v>145</v>
       </c>
       <c r="CU34" s="16" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV34" s="16" t="s">
         <v>146</v>
@@ -11124,40 +11277,43 @@
         <v>146</v>
       </c>
       <c r="CX34" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY34" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="CY34" s="16" t="s">
+      <c r="CZ34" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="CZ34" s="16" t="s">
+      <c r="DA34" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="DA34" s="16" t="s">
+      <c r="DB34" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="DB34" s="16" t="s">
-        <v>270</v>
       </c>
       <c r="DC34" s="16" t="s">
         <v>270</v>
       </c>
       <c r="DD34" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="DE34" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DE34" s="16" t="s">
+      <c r="DF34" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DF34" s="16" t="s">
+      <c r="DG34" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="DG34" s="16" t="s">
+      <c r="DH34" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DH34" s="16" t="s">
+      <c r="DI34" s="16" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="35" spans="1:112" ht="20" customHeight="1">
+    <row r="35" spans="1:113" ht="20" customHeight="1">
       <c r="B35" s="13" t="s">
         <v>107</v>
       </c>
@@ -11375,8 +11531,9 @@
       <c r="DF35" s="16"/>
       <c r="DG35" s="16"/>
       <c r="DH35" s="16"/>
+      <c r="DI35" s="16"/>
     </row>
-    <row r="36" spans="1:112" ht="20" customHeight="1">
+    <row r="36" spans="1:113" ht="20" customHeight="1">
       <c r="B36" s="13" t="s">
         <v>107</v>
       </c>
@@ -11600,8 +11757,9 @@
       <c r="DF36" s="16"/>
       <c r="DG36" s="16"/>
       <c r="DH36" s="16"/>
+      <c r="DI36" s="16"/>
     </row>
-    <row r="37" spans="1:112" ht="20" customHeight="1">
+    <row r="37" spans="1:113" ht="20" customHeight="1">
       <c r="A37" t="b">
         <v>1</v>
       </c>
@@ -11825,7 +11983,7 @@
         <v>149</v>
       </c>
       <c r="CU37" s="21" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV37" s="21" t="s">
         <v>146</v>
@@ -11834,40 +11992,43 @@
         <v>146</v>
       </c>
       <c r="CX37" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY37" s="21" t="s">
         <v>260</v>
-      </c>
-      <c r="CY37" s="21" t="s">
-        <v>261</v>
       </c>
       <c r="CZ37" s="21" t="s">
         <v>261</v>
       </c>
       <c r="DA37" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="DB37" s="21" t="s">
         <v>149</v>
-      </c>
-      <c r="DB37" s="21" t="s">
-        <v>270</v>
       </c>
       <c r="DC37" s="21" t="s">
         <v>270</v>
       </c>
       <c r="DD37" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="DE37" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="DE37" s="21" t="s">
+      <c r="DF37" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="DF37" s="21" t="s">
+      <c r="DG37" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DG37" s="22" t="s">
+      <c r="DH37" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DH37" s="22" t="s">
+      <c r="DI37" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:112" ht="20" customHeight="1">
+    <row r="38" spans="1:113" ht="20" customHeight="1">
       <c r="A38" t="b">
         <v>1</v>
       </c>
@@ -12091,7 +12252,7 @@
         <v>149</v>
       </c>
       <c r="CU38" s="26" t="s">
-        <v>146</v>
+        <v>290</v>
       </c>
       <c r="CV38" s="26" t="s">
         <v>146</v>
@@ -12100,22 +12261,22 @@
         <v>146</v>
       </c>
       <c r="CX38" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY38" s="26" t="s">
         <v>279</v>
-      </c>
-      <c r="CY38" s="26" t="s">
-        <v>280</v>
       </c>
       <c r="CZ38" s="26" t="s">
         <v>280</v>
       </c>
       <c r="DA38" s="26" t="s">
-        <v>149</v>
+        <v>280</v>
       </c>
       <c r="DB38" s="26" t="s">
         <v>149</v>
       </c>
       <c r="DC38" s="26" t="s">
-        <v>270</v>
+        <v>149</v>
       </c>
       <c r="DD38" s="26" t="s">
         <v>270</v>
@@ -12124,16 +12285,19 @@
         <v>270</v>
       </c>
       <c r="DF38" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="DG38" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DG38" s="26" t="s">
+      <c r="DH38" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DH38" s="26" t="s">
+      <c r="DI38" s="26" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="39" spans="1:112" ht="20" customHeight="1">
+    <row r="39" spans="1:113" ht="20" customHeight="1">
       <c r="B39" s="28" t="s">
         <v>107</v>
       </c>
@@ -12361,6 +12525,276 @@
       <c r="DF39" s="31"/>
       <c r="DG39" s="31"/>
       <c r="DH39" s="31"/>
+      <c r="DI39" s="31"/>
+    </row>
+    <row r="40" spans="1:113" s="49" customFormat="1" ht="20" customHeight="1">
+      <c r="A40" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="45">
+        <v>313458</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F40" s="45">
+        <v>1008743219</v>
+      </c>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="O40" s="46"/>
+      <c r="P40" s="45">
+        <v>19970619</v>
+      </c>
+      <c r="Q40" s="45"/>
+      <c r="R40" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="S40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="T40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="U40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="V40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="W40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="X40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AK40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM40" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP40" s="45">
+        <v>20170214</v>
+      </c>
+      <c r="AQ40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AR40" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS40" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AV40" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW40" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="AX40" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY40" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="AZ40" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA40" s="45">
+        <v>20170611</v>
+      </c>
+      <c r="BB40" s="45">
+        <v>344511</v>
+      </c>
+      <c r="BC40" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD40" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="BE40" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF40" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG40" s="48"/>
+      <c r="BH40" s="48"/>
+      <c r="BI40" s="48"/>
+      <c r="BJ40" s="48"/>
+      <c r="BK40" s="48"/>
+      <c r="BL40" s="48"/>
+      <c r="BM40" s="48"/>
+      <c r="BN40" s="48"/>
+      <c r="BO40" s="48"/>
+      <c r="BP40" s="48"/>
+      <c r="BQ40" s="48"/>
+      <c r="BR40" s="48"/>
+      <c r="BS40" s="48"/>
+      <c r="BT40" s="48"/>
+      <c r="BU40" s="48"/>
+      <c r="BV40" s="48"/>
+      <c r="BW40" s="48"/>
+      <c r="BX40" s="48"/>
+      <c r="BY40" s="48"/>
+      <c r="BZ40" s="48"/>
+      <c r="CA40" s="48"/>
+      <c r="CB40" s="48"/>
+      <c r="CC40" s="48"/>
+      <c r="CD40" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="CE40" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="CF40" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="CG40" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="CH40" s="48"/>
+      <c r="CI40" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="CJ40" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="CK40" s="45">
+        <v>2</v>
+      </c>
+      <c r="CL40" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="CM40" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="CN40" s="45">
+        <v>20</v>
+      </c>
+      <c r="CO40" s="48"/>
+      <c r="CP40" s="48"/>
+      <c r="CQ40" s="48"/>
+      <c r="CR40" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="CS40" s="45">
+        <v>344511</v>
+      </c>
+      <c r="CT40" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="CU40" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="CV40" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="CW40" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="CX40" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY40" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="CZ40" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="DA40" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="DB40" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="DC40" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="DD40" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="DE40" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="DF40" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="DG40" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="DH40" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="DI40" s="48" t="s">
+        <v>275</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Add "Possible Other P64 Charges" column to outputs
When the `OFFENSE_DESCR` is neither empty nor contains the string "SEE
COMMENT FOR CHARGE", we may find text matching Prop64 charges in the
`COMMENT_TEXT` column. As we cannot be sure that they should override
the charges in `OFFENSE_DESCR`, we flag them in the output.

[#167404950]

Co-authored-by: Symonne Singleton <symonne@codeforamerica.org>
</commit_message>
<xml_diff>
--- a/test_fixtures/configurable_flow.xlsx
+++ b/test_fixtures/configurable_flow.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr date1904="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christa/go/src/gogen/test_fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F0A1D8-36FC-E940-9980-70F239EC618E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26740"/>
+    <workbookView xWindow="120" yWindow="2520" windowWidth="51200" windowHeight="26740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2324" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="296">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -901,12 +907,18 @@
   </si>
   <si>
     <t>2.7</t>
+  </si>
+  <si>
+    <t>Possible Other P64 Charges</t>
+  </si>
+  <si>
+    <t>11359 HS-OTHER CANNABIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2842,19 +2854,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DI40"/>
+  <dimension ref="A1:DJ40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CJ1" workbookViewId="0">
-      <pane ySplit="1200" topLeftCell="A5" activePane="bottomLeft"/>
-      <selection activeCell="CU2" sqref="CU2"/>
-      <selection pane="bottomLeft" activeCell="DB45" sqref="DB45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CD2" workbookViewId="0">
+      <pane ySplit="1200" activePane="bottomLeft"/>
+      <selection activeCell="CU2" sqref="CU1:CU1048576"/>
+      <selection pane="bottomLeft" activeCell="CE46" sqref="CE46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
@@ -2945,17 +2957,17 @@
     <col min="95" max="95" width="26.83203125" style="1" customWidth="1"/>
     <col min="96" max="96" width="12.5" style="1" customWidth="1"/>
     <col min="97" max="97" width="29.6640625" style="1" customWidth="1"/>
-    <col min="98" max="99" width="24" style="1" customWidth="1"/>
-    <col min="100" max="102" width="23.6640625" style="1" customWidth="1"/>
-    <col min="103" max="103" width="12.5" style="1" customWidth="1"/>
-    <col min="104" max="104" width="23.5" style="1" customWidth="1"/>
-    <col min="105" max="105" width="23.1640625" style="1" customWidth="1"/>
-    <col min="106" max="110" width="20.5" style="1" customWidth="1"/>
-    <col min="111" max="112" width="25.83203125" style="1" customWidth="1"/>
-    <col min="113" max="113" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="98" max="100" width="24" style="1" customWidth="1"/>
+    <col min="101" max="103" width="23.6640625" style="1" customWidth="1"/>
+    <col min="104" max="104" width="12.5" style="1" customWidth="1"/>
+    <col min="105" max="105" width="23.5" style="1" customWidth="1"/>
+    <col min="106" max="106" width="23.1640625" style="1" customWidth="1"/>
+    <col min="107" max="111" width="20.5" style="1" customWidth="1"/>
+    <col min="112" max="113" width="25.83203125" style="1" customWidth="1"/>
+    <col min="114" max="114" width="52.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" s="42" customFormat="1" ht="27.75" customHeight="1">
+    <row r="1" spans="1:114" s="42" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="39" t="s">
         <v>253</v>
       </c>
@@ -3144,8 +3156,11 @@
       <c r="DI1" s="41" t="s">
         <v>252</v>
       </c>
+      <c r="DJ1" s="41" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="2" spans="1:113" ht="20.25" customHeight="1">
+    <row r="2" spans="1:114" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3441,52 +3456,55 @@
         <v>96</v>
       </c>
       <c r="CU2" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="CV2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="CV2" s="2" t="s">
+      <c r="CW2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="CW2" s="2" t="s">
+      <c r="CX2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="CX2" s="2" t="s">
+      <c r="CY2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="CY2" s="2" t="s">
+      <c r="CZ2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="CZ2" s="2" t="s">
+      <c r="DA2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="DA2" s="2" t="s">
+      <c r="DB2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="DB2" s="2" t="s">
+      <c r="DC2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="DC2" s="2" t="s">
+      <c r="DD2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="DD2" s="2" t="s">
+      <c r="DE2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="DE2" s="2" t="s">
+      <c r="DF2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="DF2" s="2" t="s">
+      <c r="DG2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="DG2" s="2" t="s">
+      <c r="DH2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="DH2" s="2" t="s">
+      <c r="DI2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="DI2" s="2" t="s">
+      <c r="DJ2" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:113" ht="20.25" customHeight="1">
+    <row r="3" spans="1:114" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>107</v>
       </c>
@@ -3704,11 +3722,12 @@
       <c r="DD3" s="6"/>
       <c r="DE3" s="6"/>
       <c r="DF3" s="6"/>
-      <c r="DG3" s="7"/>
+      <c r="DG3" s="6"/>
       <c r="DH3" s="7"/>
       <c r="DI3" s="7"/>
+      <c r="DJ3" s="7"/>
     </row>
-    <row r="4" spans="1:113" ht="20" customHeight="1">
+    <row r="4" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
         <v>107</v>
       </c>
@@ -3936,11 +3955,12 @@
       <c r="DD4" s="11"/>
       <c r="DE4" s="11"/>
       <c r="DF4" s="11"/>
-      <c r="DG4" s="12"/>
+      <c r="DG4" s="11"/>
       <c r="DH4" s="12"/>
       <c r="DI4" s="12"/>
+      <c r="DJ4" s="12"/>
     </row>
-    <row r="5" spans="1:113" ht="20" customHeight="1">
+    <row r="5" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="8" t="s">
         <v>107</v>
       </c>
@@ -4158,11 +4178,12 @@
       <c r="DD5" s="11"/>
       <c r="DE5" s="11"/>
       <c r="DF5" s="11"/>
-      <c r="DG5" s="12"/>
+      <c r="DG5" s="11"/>
       <c r="DH5" s="12"/>
       <c r="DI5" s="12"/>
+      <c r="DJ5" s="12"/>
     </row>
-    <row r="6" spans="1:113" ht="20" customHeight="1">
+    <row r="6" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4380,11 +4401,12 @@
       <c r="DD6" s="11"/>
       <c r="DE6" s="11"/>
       <c r="DF6" s="11"/>
-      <c r="DG6" s="12"/>
+      <c r="DG6" s="11"/>
       <c r="DH6" s="12"/>
       <c r="DI6" s="12"/>
+      <c r="DJ6" s="12"/>
     </row>
-    <row r="7" spans="1:113" ht="20" customHeight="1">
+    <row r="7" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="8" t="s">
         <v>107</v>
       </c>
@@ -4602,11 +4624,12 @@
       <c r="DD7" s="11"/>
       <c r="DE7" s="11"/>
       <c r="DF7" s="11"/>
-      <c r="DG7" s="12"/>
+      <c r="DG7" s="11"/>
       <c r="DH7" s="12"/>
       <c r="DI7" s="12"/>
+      <c r="DJ7" s="12"/>
     </row>
-    <row r="8" spans="1:113" ht="20" customHeight="1">
+    <row r="8" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -4829,11 +4852,9 @@
       <c r="CT8" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="CU8" s="11" t="s">
+      <c r="CU8" s="11"/>
+      <c r="CV8" s="11" t="s">
         <v>290</v>
-      </c>
-      <c r="CV8" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="CW8" s="11" t="s">
         <v>146</v>
@@ -4842,40 +4863,43 @@
         <v>146</v>
       </c>
       <c r="CY8" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ8" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="CZ8" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="DA8" s="11" t="s">
         <v>148</v>
       </c>
       <c r="DB8" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="DC8" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="DC8" s="11" t="s">
+      <c r="DD8" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="DD8" s="11" t="s">
+      <c r="DE8" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="DE8" s="11" t="s">
-        <v>270</v>
       </c>
       <c r="DF8" s="11" t="s">
         <v>270</v>
       </c>
       <c r="DG8" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="DH8" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="DH8" s="11" t="s">
+      <c r="DI8" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="DI8" s="11" t="s">
+      <c r="DJ8" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:113" ht="20" customHeight="1">
+    <row r="9" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="23" t="s">
         <v>107</v>
       </c>
@@ -5096,8 +5120,9 @@
       <c r="DG9" s="26"/>
       <c r="DH9" s="26"/>
       <c r="DI9" s="26"/>
+      <c r="DJ9" s="26"/>
     </row>
-    <row r="10" spans="1:113" ht="20" customHeight="1">
+    <row r="10" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -5320,53 +5345,54 @@
       <c r="CT10" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="CU10" s="26" t="s">
+      <c r="CU10" s="26"/>
+      <c r="CV10" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="CV10" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CW10" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CX10" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY10" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="CY10" s="26" t="s">
+      <c r="CZ10" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="CZ10" s="26" t="s">
+      <c r="DA10" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="DA10" s="26" t="s">
+      <c r="DB10" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="DB10" s="26" t="s">
+      <c r="DC10" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="DC10" s="26" t="s">
+      <c r="DD10" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DD10" s="26" t="s">
+      <c r="DE10" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DE10" s="26" t="s">
+      <c r="DF10" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DF10" s="26" t="s">
+      <c r="DG10" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DG10" s="26" t="s">
+      <c r="DH10" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DH10" s="26" t="s">
+      <c r="DI10" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DI10" s="26" t="s">
+      <c r="DJ10" s="26" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:113" ht="20" customHeight="1">
+    <row r="11" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="23" t="s">
         <v>107</v>
       </c>
@@ -5583,8 +5609,9 @@
       <c r="DG11" s="26"/>
       <c r="DH11" s="26"/>
       <c r="DI11" s="26"/>
+      <c r="DJ11" s="26"/>
     </row>
-    <row r="12" spans="1:113" ht="20" customHeight="1">
+    <row r="12" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -5807,53 +5834,54 @@
       <c r="CT12" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="CU12" s="26" t="s">
+      <c r="CU12" s="26"/>
+      <c r="CV12" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="CV12" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CW12" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CX12" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CY12" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="CY12" s="26" t="s">
+      <c r="CZ12" s="26" t="s">
         <v>256</v>
-      </c>
-      <c r="CZ12" s="26" t="s">
-        <v>255</v>
       </c>
       <c r="DA12" s="26" t="s">
         <v>255</v>
       </c>
       <c r="DB12" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="DC12" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="DC12" s="26" t="s">
+      <c r="DD12" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DD12" s="26" t="s">
+      <c r="DE12" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DE12" s="26" t="s">
+      <c r="DF12" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DF12" s="26" t="s">
+      <c r="DG12" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DG12" s="26" t="s">
+      <c r="DH12" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DH12" s="26" t="s">
+      <c r="DI12" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DI12" s="26" t="s">
+      <c r="DJ12" s="26" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="13" spans="1:113" ht="20" customHeight="1">
+    <row r="13" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="23" t="s">
         <v>107</v>
       </c>
@@ -6078,8 +6106,9 @@
       <c r="DG13" s="26"/>
       <c r="DH13" s="26"/>
       <c r="DI13" s="26"/>
+      <c r="DJ13" s="26"/>
     </row>
-    <row r="14" spans="1:113" ht="20" customHeight="1">
+    <row r="14" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="b">
         <v>1</v>
       </c>
@@ -6304,11 +6333,9 @@
       <c r="CT14" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="CU14" s="16" t="s">
+      <c r="CU14" s="16"/>
+      <c r="CV14" s="16" t="s">
         <v>290</v>
-      </c>
-      <c r="CV14" s="16" t="s">
-        <v>146</v>
       </c>
       <c r="CW14" s="16" t="s">
         <v>146</v>
@@ -6317,40 +6344,43 @@
         <v>146</v>
       </c>
       <c r="CY14" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ14" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="CZ14" s="16" t="s">
+      <c r="DA14" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="DA14" s="16" t="s">
+      <c r="DB14" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="DB14" s="16" t="s">
+      <c r="DC14" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="DC14" s="16" t="s">
+      <c r="DD14" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DD14" s="16" t="s">
+      <c r="DE14" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="DE14" s="16" t="s">
+      <c r="DF14" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DF14" s="16" t="s">
+      <c r="DG14" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DG14" s="16" t="s">
+      <c r="DH14" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DH14" s="17" t="s">
+      <c r="DI14" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="DI14" s="17" t="s">
+      <c r="DJ14" s="17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:113" ht="20" customHeight="1">
+    <row r="15" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="13" t="s">
         <v>107</v>
       </c>
@@ -6560,13 +6590,17 @@
       </c>
       <c r="CO15" s="17"/>
       <c r="CP15" s="17"/>
-      <c r="CQ15" s="17"/>
+      <c r="CQ15" s="17" t="s">
+        <v>295</v>
+      </c>
       <c r="CR15" s="16" t="s">
         <v>108</v>
       </c>
       <c r="CS15" s="17"/>
       <c r="CT15" s="16"/>
-      <c r="CU15" s="16"/>
+      <c r="CU15" s="16" t="s">
+        <v>295</v>
+      </c>
       <c r="CV15" s="16"/>
       <c r="CW15" s="16"/>
       <c r="CX15" s="16"/>
@@ -6578,11 +6612,12 @@
       <c r="DD15" s="16"/>
       <c r="DE15" s="16"/>
       <c r="DF15" s="16"/>
-      <c r="DG15" s="17"/>
+      <c r="DG15" s="16"/>
       <c r="DH15" s="17"/>
       <c r="DI15" s="17"/>
+      <c r="DJ15" s="17"/>
     </row>
-    <row r="16" spans="1:113" ht="20" customHeight="1">
+    <row r="16" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="13" t="s">
         <v>107</v>
       </c>
@@ -6810,11 +6845,12 @@
       <c r="DD16" s="16"/>
       <c r="DE16" s="16"/>
       <c r="DF16" s="16"/>
-      <c r="DG16" s="17"/>
+      <c r="DG16" s="16"/>
       <c r="DH16" s="17"/>
       <c r="DI16" s="17"/>
+      <c r="DJ16" s="17"/>
     </row>
-    <row r="17" spans="1:113" ht="20" customHeight="1">
+    <row r="17" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -7037,11 +7073,9 @@
       <c r="CT17" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="CU17" s="16" t="s">
+      <c r="CU17" s="16"/>
+      <c r="CV17" s="16" t="s">
         <v>290</v>
-      </c>
-      <c r="CV17" s="16" t="s">
-        <v>146</v>
       </c>
       <c r="CW17" s="16" t="s">
         <v>146</v>
@@ -7050,40 +7084,43 @@
         <v>146</v>
       </c>
       <c r="CY17" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ17" s="16" t="s">
         <v>258</v>
-      </c>
-      <c r="CZ17" s="16" t="s">
-        <v>257</v>
       </c>
       <c r="DA17" s="16" t="s">
         <v>257</v>
       </c>
       <c r="DB17" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="DC17" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="DC17" s="16" t="s">
+      <c r="DD17" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DD17" s="16" t="s">
+      <c r="DE17" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="DE17" s="16" t="s">
+      <c r="DF17" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DF17" s="16" t="s">
+      <c r="DG17" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DG17" s="16" t="s">
+      <c r="DH17" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="DH17" s="17" t="s">
+      <c r="DI17" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="DI17" s="17" t="s">
+      <c r="DJ17" s="17" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="18" spans="1:113" ht="20" customHeight="1">
+    <row r="18" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="13" t="s">
         <v>107</v>
       </c>
@@ -7309,11 +7346,12 @@
       <c r="DD18" s="16"/>
       <c r="DE18" s="16"/>
       <c r="DF18" s="16"/>
-      <c r="DG18" s="17"/>
+      <c r="DG18" s="16"/>
       <c r="DH18" s="17"/>
       <c r="DI18" s="17"/>
+      <c r="DJ18" s="17"/>
     </row>
-    <row r="19" spans="1:113" ht="20" customHeight="1">
+    <row r="19" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
@@ -7541,11 +7579,12 @@
       <c r="DD19" s="21"/>
       <c r="DE19" s="21"/>
       <c r="DF19" s="21"/>
-      <c r="DG19" s="22"/>
+      <c r="DG19" s="21"/>
       <c r="DH19" s="22"/>
       <c r="DI19" s="22"/>
+      <c r="DJ19" s="22"/>
     </row>
-    <row r="20" spans="1:113" ht="20" customHeight="1">
+    <row r="20" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="b">
         <v>1</v>
       </c>
@@ -7762,53 +7801,54 @@
       <c r="CT20" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="CU20" s="21" t="s">
+      <c r="CU20" s="21"/>
+      <c r="CV20" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="CV20" s="21" t="s">
+      <c r="CW20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CW20" s="21" t="s">
+      <c r="CX20" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="CX20" s="21" t="s">
+      <c r="CY20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CY20" s="21" t="s">
+      <c r="CZ20" s="21" t="s">
         <v>266</v>
-      </c>
-      <c r="CZ20" s="21" t="s">
-        <v>267</v>
       </c>
       <c r="DA20" s="21" t="s">
         <v>267</v>
       </c>
       <c r="DB20" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="DC20" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="DC20" s="21" t="s">
+      <c r="DD20" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="DD20" s="21" t="s">
-        <v>149</v>
       </c>
       <c r="DE20" s="21" t="s">
         <v>149</v>
       </c>
       <c r="DF20" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DG20" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="DG20" s="21" t="s">
+      <c r="DH20" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DH20" s="22" t="s">
+      <c r="DI20" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DI20" s="22" t="s">
+      <c r="DJ20" s="22" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="1:113" ht="20" customHeight="1">
+    <row r="21" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="18" t="s">
         <v>107</v>
       </c>
@@ -8036,11 +8076,12 @@
       <c r="DD21" s="21"/>
       <c r="DE21" s="21"/>
       <c r="DF21" s="21"/>
-      <c r="DG21" s="22"/>
+      <c r="DG21" s="21"/>
       <c r="DH21" s="22"/>
       <c r="DI21" s="22"/>
+      <c r="DJ21" s="22"/>
     </row>
-    <row r="22" spans="1:113" ht="20" customHeight="1">
+    <row r="22" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="b">
         <v>1</v>
       </c>
@@ -8263,53 +8304,54 @@
       <c r="CT22" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="CU22" s="21" t="s">
+      <c r="CU22" s="21"/>
+      <c r="CV22" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="CV22" s="21" t="s">
+      <c r="CW22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CW22" s="21" t="s">
+      <c r="CX22" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="CX22" s="21" t="s">
+      <c r="CY22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="CY22" s="21" t="s">
+      <c r="CZ22" s="21" t="s">
         <v>266</v>
-      </c>
-      <c r="CZ22" s="21" t="s">
-        <v>267</v>
       </c>
       <c r="DA22" s="21" t="s">
         <v>267</v>
       </c>
       <c r="DB22" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="DC22" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="DC22" s="21" t="s">
+      <c r="DD22" s="21" t="s">
         <v>270</v>
-      </c>
-      <c r="DD22" s="21" t="s">
-        <v>149</v>
       </c>
       <c r="DE22" s="21" t="s">
         <v>149</v>
       </c>
       <c r="DF22" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="DG22" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="DG22" s="21" t="s">
+      <c r="DH22" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DH22" s="22" t="s">
+      <c r="DI22" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DI22" s="22" t="s">
+      <c r="DJ22" s="22" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:113" ht="20" customHeight="1">
+    <row r="23" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -8528,32 +8570,30 @@
       <c r="CT23" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="CU23" s="26" t="s">
+      <c r="CU23" s="26"/>
+      <c r="CV23" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="CV23" s="26" t="s">
+      <c r="CW23" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="CW23" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CX23" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CY23" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ23" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="CZ23" s="26" t="s">
+      <c r="DA23" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="DA23" s="26" t="s">
+      <c r="DB23" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="DB23" s="26" t="s">
+      <c r="DC23" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="DC23" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="DD23" s="26" t="s">
         <v>149</v>
@@ -8562,19 +8602,22 @@
         <v>149</v>
       </c>
       <c r="DF23" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DG23" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DG23" s="26" t="s">
+      <c r="DH23" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DH23" s="27" t="s">
+      <c r="DI23" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="DI23" s="27" t="s">
+      <c r="DJ23" s="27" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="24" spans="1:113" ht="20" customHeight="1">
+    <row r="24" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="23" t="s">
         <v>107</v>
       </c>
@@ -8798,11 +8841,12 @@
       <c r="DD24" s="26"/>
       <c r="DE24" s="26"/>
       <c r="DF24" s="26"/>
-      <c r="DG24" s="27"/>
+      <c r="DG24" s="26"/>
       <c r="DH24" s="27"/>
       <c r="DI24" s="27"/>
+      <c r="DJ24" s="27"/>
     </row>
-    <row r="25" spans="1:113" ht="20" customHeight="1">
+    <row r="25" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="23" t="s">
         <v>107</v>
       </c>
@@ -9012,11 +9056,12 @@
       <c r="DD25" s="26"/>
       <c r="DE25" s="26"/>
       <c r="DF25" s="26"/>
-      <c r="DG25" s="27"/>
+      <c r="DG25" s="26"/>
       <c r="DH25" s="27"/>
       <c r="DI25" s="27"/>
+      <c r="DJ25" s="27"/>
     </row>
-    <row r="26" spans="1:113" ht="20" customHeight="1">
+    <row r="26" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="b">
         <v>1</v>
       </c>
@@ -9223,32 +9268,30 @@
       <c r="CT26" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="CU26" s="26" t="s">
+      <c r="CU26" s="26"/>
+      <c r="CV26" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="CV26" s="26" t="s">
+      <c r="CW26" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="CW26" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CX26" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CY26" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ26" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="CZ26" s="26" t="s">
+      <c r="DA26" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="DA26" s="26" t="s">
+      <c r="DB26" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="DB26" s="26" t="s">
+      <c r="DC26" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="DC26" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="DD26" s="26" t="s">
         <v>149</v>
@@ -9257,19 +9300,22 @@
         <v>149</v>
       </c>
       <c r="DF26" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DG26" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DG26" s="26" t="s">
+      <c r="DH26" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DH26" s="26" t="s">
+      <c r="DI26" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DI26" s="26" t="s">
+      <c r="DJ26" s="26" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:113" ht="20" customHeight="1">
+    <row r="27" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="b">
         <v>1</v>
       </c>
@@ -9476,32 +9522,30 @@
       <c r="CT27" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="CU27" s="26" t="s">
+      <c r="CU27" s="26"/>
+      <c r="CV27" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="CV27" s="26" t="s">
+      <c r="CW27" s="26" t="s">
         <v>190</v>
-      </c>
-      <c r="CW27" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CX27" s="26" t="s">
         <v>146</v>
       </c>
       <c r="CY27" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ27" s="26" t="s">
         <v>199</v>
-      </c>
-      <c r="CZ27" s="26" t="s">
-        <v>193</v>
       </c>
       <c r="DA27" s="26" t="s">
         <v>193</v>
       </c>
       <c r="DB27" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="DC27" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="DC27" s="26" t="s">
-        <v>149</v>
       </c>
       <c r="DD27" s="26" t="s">
         <v>149</v>
@@ -9510,19 +9554,22 @@
         <v>149</v>
       </c>
       <c r="DF27" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="DG27" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DG27" s="26" t="s">
+      <c r="DH27" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DH27" s="26" t="s">
+      <c r="DI27" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="DI27" s="26" t="s">
+      <c r="DJ27" s="26" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:113" ht="20" customHeight="1">
+    <row r="28" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="b">
         <v>1</v>
       </c>
@@ -9745,11 +9792,9 @@
       <c r="CT28" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="CU28" s="31" t="s">
+      <c r="CU28" s="31"/>
+      <c r="CV28" s="31" t="s">
         <v>290</v>
-      </c>
-      <c r="CV28" s="31" t="s">
-        <v>146</v>
       </c>
       <c r="CW28" s="31" t="s">
         <v>146</v>
@@ -9758,40 +9803,43 @@
         <v>146</v>
       </c>
       <c r="CY28" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ28" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="CZ28" s="31" t="s">
+      <c r="DA28" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="DA28" s="31" t="s">
+      <c r="DB28" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="DB28" s="31" t="s">
+      <c r="DC28" s="31" t="s">
         <v>156</v>
-      </c>
-      <c r="DC28" s="31" t="s">
-        <v>270</v>
       </c>
       <c r="DD28" s="31" t="s">
         <v>270</v>
       </c>
       <c r="DE28" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="DF28" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="DF28" s="31" t="s">
+      <c r="DG28" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="DG28" s="31" t="s">
+      <c r="DH28" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="DH28" s="31" t="s">
+      <c r="DI28" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="DI28" s="31" t="s">
+      <c r="DJ28" s="31" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:113" ht="20" customHeight="1">
+    <row r="29" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="28" t="s">
         <v>107</v>
       </c>
@@ -10019,11 +10067,12 @@
       <c r="DD29" s="31"/>
       <c r="DE29" s="31"/>
       <c r="DF29" s="31"/>
-      <c r="DG29" s="32"/>
+      <c r="DG29" s="31"/>
       <c r="DH29" s="32"/>
       <c r="DI29" s="32"/>
+      <c r="DJ29" s="32"/>
     </row>
-    <row r="30" spans="1:113" ht="20" customHeight="1">
+    <row r="30" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="b">
         <v>1</v>
       </c>
@@ -10246,11 +10295,9 @@
       <c r="CT30" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="CU30" s="31" t="s">
+      <c r="CU30" s="31"/>
+      <c r="CV30" s="31" t="s">
         <v>290</v>
-      </c>
-      <c r="CV30" s="31" t="s">
-        <v>146</v>
       </c>
       <c r="CW30" s="31" t="s">
         <v>146</v>
@@ -10259,40 +10306,43 @@
         <v>146</v>
       </c>
       <c r="CY30" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ30" s="31" t="s">
         <v>208</v>
-      </c>
-      <c r="CZ30" s="31" t="s">
-        <v>206</v>
       </c>
       <c r="DA30" s="31" t="s">
         <v>206</v>
       </c>
       <c r="DB30" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="DC30" s="31" t="s">
         <v>156</v>
-      </c>
-      <c r="DC30" s="31" t="s">
-        <v>270</v>
       </c>
       <c r="DD30" s="31" t="s">
         <v>270</v>
       </c>
       <c r="DE30" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="DF30" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="DF30" s="31" t="s">
+      <c r="DG30" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="DG30" s="31" t="s">
+      <c r="DH30" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="DH30" s="31" t="s">
+      <c r="DI30" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="DI30" s="31" t="s">
+      <c r="DJ30" s="31" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:113" ht="20" customHeight="1">
+    <row r="31" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="b">
         <v>1</v>
       </c>
@@ -10515,53 +10565,54 @@
       <c r="CT31" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="CU31" s="11" t="s">
+      <c r="CU31" s="11"/>
+      <c r="CV31" s="11" t="s">
         <v>290</v>
       </c>
-      <c r="CV31" s="11" t="s">
+      <c r="CW31" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="CW31" s="11" t="s">
-        <v>146</v>
       </c>
       <c r="CX31" s="11" t="s">
         <v>146</v>
       </c>
       <c r="CY31" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ31" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="CZ31" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="DA31" s="11" t="s">
         <v>205</v>
       </c>
       <c r="DB31" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="DC31" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="DC31" s="11" t="s">
+      <c r="DD31" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="DD31" s="11" t="s">
+      <c r="DE31" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="DE31" s="11" t="s">
-        <v>270</v>
       </c>
       <c r="DF31" s="11" t="s">
         <v>270</v>
       </c>
       <c r="DG31" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="DH31" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="DH31" s="11" t="s">
+      <c r="DI31" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="DI31" s="11" t="s">
+      <c r="DJ31" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:113" ht="20" customHeight="1">
+    <row r="32" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="8" t="s">
         <v>107</v>
       </c>
@@ -10789,11 +10840,12 @@
       <c r="DD32" s="11"/>
       <c r="DE32" s="11"/>
       <c r="DF32" s="11"/>
-      <c r="DG32" s="12"/>
+      <c r="DG32" s="11"/>
       <c r="DH32" s="12"/>
       <c r="DI32" s="12"/>
+      <c r="DJ32" s="12"/>
     </row>
-    <row r="33" spans="1:113" ht="20" customHeight="1">
+    <row r="33" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="b">
         <v>1</v>
       </c>
@@ -11006,11 +11058,9 @@
       <c r="CT33" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="CU33" s="26" t="s">
+      <c r="CU33" s="26"/>
+      <c r="CV33" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="CV33" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CW33" s="26" t="s">
         <v>146</v>
@@ -11019,40 +11069,43 @@
         <v>146</v>
       </c>
       <c r="CY33" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ33" s="26" t="s">
         <v>215</v>
-      </c>
-      <c r="CZ33" s="26" t="s">
-        <v>216</v>
       </c>
       <c r="DA33" s="26" t="s">
         <v>216</v>
       </c>
       <c r="DB33" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="DC33" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="DC33" s="26" t="s">
+      <c r="DD33" s="26" t="s">
         <v>270</v>
       </c>
-      <c r="DD33" s="26" t="s">
+      <c r="DE33" s="26" t="s">
         <v>149</v>
-      </c>
-      <c r="DE33" s="26" t="s">
-        <v>270</v>
       </c>
       <c r="DF33" s="26" t="s">
         <v>270</v>
       </c>
       <c r="DG33" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="DH33" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DH33" s="26" t="s">
+      <c r="DI33" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DI33" s="26" t="s">
+      <c r="DJ33" s="26" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:113" ht="20" customHeight="1">
+    <row r="34" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="b">
         <v>1</v>
       </c>
@@ -11267,11 +11320,9 @@
       <c r="CT34" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="CU34" s="16" t="s">
+      <c r="CU34" s="16"/>
+      <c r="CV34" s="16" t="s">
         <v>290</v>
-      </c>
-      <c r="CV34" s="16" t="s">
-        <v>146</v>
       </c>
       <c r="CW34" s="16" t="s">
         <v>146</v>
@@ -11280,40 +11331,43 @@
         <v>146</v>
       </c>
       <c r="CY34" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ34" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="CZ34" s="16" t="s">
+      <c r="DA34" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="DA34" s="16" t="s">
+      <c r="DB34" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="DB34" s="16" t="s">
+      <c r="DC34" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="DC34" s="16" t="s">
-        <v>270</v>
       </c>
       <c r="DD34" s="16" t="s">
         <v>270</v>
       </c>
       <c r="DE34" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="DF34" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="DF34" s="16" t="s">
+      <c r="DG34" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="DG34" s="16" t="s">
+      <c r="DH34" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="DH34" s="16" t="s">
+      <c r="DI34" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="DI34" s="16" t="s">
+      <c r="DJ34" s="16" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="35" spans="1:113" ht="20" customHeight="1">
+    <row r="35" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="13" t="s">
         <v>107</v>
       </c>
@@ -11532,8 +11586,9 @@
       <c r="DG35" s="16"/>
       <c r="DH35" s="16"/>
       <c r="DI35" s="16"/>
+      <c r="DJ35" s="16"/>
     </row>
-    <row r="36" spans="1:113" ht="20" customHeight="1">
+    <row r="36" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="13" t="s">
         <v>107</v>
       </c>
@@ -11758,8 +11813,9 @@
       <c r="DG36" s="16"/>
       <c r="DH36" s="16"/>
       <c r="DI36" s="16"/>
+      <c r="DJ36" s="16"/>
     </row>
-    <row r="37" spans="1:113" ht="20" customHeight="1">
+    <row r="37" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="b">
         <v>1</v>
       </c>
@@ -11982,11 +12038,9 @@
       <c r="CT37" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="CU37" s="21" t="s">
+      <c r="CU37" s="21"/>
+      <c r="CV37" s="21" t="s">
         <v>290</v>
-      </c>
-      <c r="CV37" s="21" t="s">
-        <v>146</v>
       </c>
       <c r="CW37" s="21" t="s">
         <v>146</v>
@@ -11995,40 +12049,43 @@
         <v>146</v>
       </c>
       <c r="CY37" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ37" s="21" t="s">
         <v>260</v>
-      </c>
-      <c r="CZ37" s="21" t="s">
-        <v>261</v>
       </c>
       <c r="DA37" s="21" t="s">
         <v>261</v>
       </c>
       <c r="DB37" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="DC37" s="21" t="s">
         <v>149</v>
-      </c>
-      <c r="DC37" s="21" t="s">
-        <v>270</v>
       </c>
       <c r="DD37" s="21" t="s">
         <v>270</v>
       </c>
       <c r="DE37" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="DF37" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="DF37" s="21" t="s">
+      <c r="DG37" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="DG37" s="21" t="s">
+      <c r="DH37" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="DH37" s="22" t="s">
+      <c r="DI37" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="DI37" s="22" t="s">
+      <c r="DJ37" s="22" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:113" ht="20" customHeight="1">
+    <row r="38" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="b">
         <v>1</v>
       </c>
@@ -12251,11 +12308,9 @@
       <c r="CT38" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="CU38" s="26" t="s">
+      <c r="CU38" s="26"/>
+      <c r="CV38" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="CV38" s="26" t="s">
-        <v>146</v>
       </c>
       <c r="CW38" s="26" t="s">
         <v>146</v>
@@ -12264,22 +12319,22 @@
         <v>146</v>
       </c>
       <c r="CY38" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ38" s="26" t="s">
         <v>279</v>
-      </c>
-      <c r="CZ38" s="26" t="s">
-        <v>280</v>
       </c>
       <c r="DA38" s="26" t="s">
         <v>280</v>
       </c>
       <c r="DB38" s="26" t="s">
-        <v>149</v>
+        <v>280</v>
       </c>
       <c r="DC38" s="26" t="s">
         <v>149</v>
       </c>
       <c r="DD38" s="26" t="s">
-        <v>270</v>
+        <v>149</v>
       </c>
       <c r="DE38" s="26" t="s">
         <v>270</v>
@@ -12288,16 +12343,19 @@
         <v>270</v>
       </c>
       <c r="DG38" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="DH38" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="DH38" s="26" t="s">
+      <c r="DI38" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="DI38" s="26" t="s">
+      <c r="DJ38" s="26" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="39" spans="1:113" ht="20" customHeight="1">
+    <row r="39" spans="1:114" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="28" t="s">
         <v>107</v>
       </c>
@@ -12526,8 +12584,9 @@
       <c r="DG39" s="31"/>
       <c r="DH39" s="31"/>
       <c r="DI39" s="31"/>
+      <c r="DJ39" s="31"/>
     </row>
-    <row r="40" spans="1:113" s="49" customFormat="1" ht="20" customHeight="1">
+    <row r="40" spans="1:114" s="49" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="49" t="b">
         <v>1</v>
       </c>
@@ -12750,11 +12809,9 @@
       <c r="CT40" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="CU40" s="46" t="s">
+      <c r="CU40" s="46"/>
+      <c r="CV40" s="46" t="s">
         <v>164</v>
-      </c>
-      <c r="CV40" s="46" t="s">
-        <v>146</v>
       </c>
       <c r="CW40" s="46" t="s">
         <v>146</v>
@@ -12763,36 +12820,39 @@
         <v>146</v>
       </c>
       <c r="CY40" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="CZ40" s="46" t="s">
         <v>292</v>
-      </c>
-      <c r="CZ40" s="46" t="s">
-        <v>293</v>
       </c>
       <c r="DA40" s="46" t="s">
         <v>293</v>
       </c>
       <c r="DB40" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="DC40" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="DC40" s="46" t="s">
+      <c r="DD40" s="46" t="s">
         <v>270</v>
       </c>
-      <c r="DD40" s="46" t="s">
+      <c r="DE40" s="46" t="s">
         <v>149</v>
-      </c>
-      <c r="DE40" s="46" t="s">
-        <v>270</v>
       </c>
       <c r="DF40" s="46" t="s">
         <v>270</v>
       </c>
       <c r="DG40" s="46" t="s">
+        <v>270</v>
+      </c>
+      <c r="DH40" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="DH40" s="46" t="s">
+      <c r="DI40" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="DI40" s="48" t="s">
+      <c r="DJ40" s="48" t="s">
         <v>275</v>
       </c>
     </row>

</xml_diff>